<commit_message>
Update course allocation template
</commit_message>
<xml_diff>
--- a/Course allocation template.xlsx
+++ b/Course allocation template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chloe\Documents\Analyses\CEGEP-CI-CalculatoR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3707053C-EC83-450A-98E9-54AD684950EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA83CFE-24FB-4616-99E1-76F7C9C34A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1FC63239-0B51-47A0-B8FF-FB9DFE3E6A3B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{1FC63239-0B51-47A0-B8FF-FB9DFE3E6A3B}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Code</t>
   </si>
@@ -73,7 +73,19 @@
     <t>First Name</t>
   </si>
   <si>
-    <t>Teacher Last Name</t>
+    <t>Scenario 1</t>
+  </si>
+  <si>
+    <t>Scenario 2</t>
+  </si>
+  <si>
+    <t>Scenario 3</t>
+  </si>
+  <si>
+    <t>Scenario 4</t>
+  </si>
+  <si>
+    <t>Scenario 5</t>
   </si>
 </sst>
 </file>
@@ -470,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1C9E49-20E5-4650-88BF-E0A3A451D972}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
@@ -480,9 +492,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E09D3576-105A-469D-87B8-FE500BE30CD5}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -496,11 +508,11 @@
     <col min="5" max="5" width="8.7265625" style="1"/>
     <col min="6" max="6" width="17.08984375" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.7265625" style="1"/>
-    <col min="8" max="8" width="21.08984375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="1"/>
+    <col min="8" max="12" width="10.1796875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -522,8 +534,20 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -546,7 +570,8 @@
     <col min="2" max="2" width="15.6328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.36328125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625" style="1"/>
+    <col min="5" max="14" width="10.1796875" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>